<commit_message>
I.A - Documentación requerimientos
</commit_message>
<xml_diff>
--- a/trunk/prograWebII/TPFinal/requerimiento/docs/Datos-TP.xlsx
+++ b/trunk/prograWebII/TPFinal/requerimiento/docs/Datos-TP.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3286" uniqueCount="333">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3286" uniqueCount="335">
   <si>
     <t>Ciudad</t>
   </si>
@@ -1023,6 +1023,12 @@
   </si>
   <si>
     <t>EMB-120</t>
+  </si>
+  <si>
+    <t>Precio Primera</t>
+  </si>
+  <si>
+    <t>Precio Economy</t>
   </si>
 </sst>
 </file>
@@ -2875,7 +2881,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F2" sqref="F2"/>
+      <selection pane="bottomLeft" activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -2884,6 +2890,8 @@
     <col min="3" max="3" width="16.85546875" customWidth="1"/>
     <col min="4" max="4" width="34.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.42578125" customWidth="1"/>
+    <col min="7" max="7" width="17.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
@@ -2899,10 +2907,10 @@
         <v>328</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>317</v>
+        <v>333</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>314</v>
+        <v>334</v>
       </c>
       <c r="H1" s="4" t="s">
         <v>320</v>
@@ -14386,7 +14394,7 @@
   <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>

</xml_diff>

<commit_message>
26/10/2014 irene.alessandrello 2)Datos-TP.xls Se quitan los tildes de las desc de ciudad TO_DO: Usar htmlcodes para las palabras con tilde
</commit_message>
<xml_diff>
--- a/trunk/prograWebII/TPFinal/requerimiento/docs/Datos-TP.xlsx
+++ b/trunk/prograWebII/TPFinal/requerimiento/docs/Datos-TP.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20430" windowHeight="7755" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20430" windowHeight="7755" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Aeropuertos" sheetId="2" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4274" uniqueCount="355">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4274" uniqueCount="380">
   <si>
     <t>Ciudad</t>
   </si>
@@ -1092,6 +1092,81 @@
   </si>
   <si>
     <t>avion_col_primera</t>
+  </si>
+  <si>
+    <t>Alto Rio Senguer</t>
+  </si>
+  <si>
+    <t>Bahia Blanca</t>
+  </si>
+  <si>
+    <t>Bolivar</t>
+  </si>
+  <si>
+    <t>Isla Martin Garcia</t>
+  </si>
+  <si>
+    <t>Junin</t>
+  </si>
+  <si>
+    <t>Olavarria</t>
+  </si>
+  <si>
+    <t>Rio Cuarto</t>
+  </si>
+  <si>
+    <t>Rio Gallegos</t>
+  </si>
+  <si>
+    <t>Rio Grande</t>
+  </si>
+  <si>
+    <t>Rio Turbio</t>
+  </si>
+  <si>
+    <t>San Martin de los Andes</t>
+  </si>
+  <si>
+    <t>Termas de Rio Hondo</t>
+  </si>
+  <si>
+    <t>Coronel Suarez</t>
+  </si>
+  <si>
+    <t>Parana</t>
+  </si>
+  <si>
+    <t>Puerto San Julian</t>
+  </si>
+  <si>
+    <t>San Miguel de Tucuman</t>
+  </si>
+  <si>
+    <t>Jose C. Paz</t>
+  </si>
+  <si>
+    <t>Neuquen</t>
+  </si>
+  <si>
+    <t>Cordoba</t>
+  </si>
+  <si>
+    <t>El Bolson</t>
+  </si>
+  <si>
+    <t>Moron</t>
+  </si>
+  <si>
+    <t>Pehuajo</t>
+  </si>
+  <si>
+    <t>San Ramon de la Nueva Oran</t>
+  </si>
+  <si>
+    <t>Curuzu Cuatia</t>
+  </si>
+  <si>
+    <t>Puerto Iguazu</t>
   </si>
 </sst>
 </file>
@@ -1321,12 +1396,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1337,6 +1406,12 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1626,7 +1701,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -3064,14 +3139,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="22" t="s">
         <v>318</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="15" t="s">
+      <c r="B1" s="22"/>
+      <c r="C1" s="23" t="s">
         <v>319</v>
       </c>
-      <c r="D1" s="15"/>
+      <c r="D1" s="23"/>
       <c r="E1" s="4" t="s">
         <v>328</v>
       </c>
@@ -14743,9 +14818,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E98"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A80" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D2" sqref="D2:D98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -14756,29 +14831,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A1" s="18"/>
-      <c r="B1" s="19" t="s">
+      <c r="A1" s="16"/>
+      <c r="B1" s="17" t="s">
         <v>335</v>
       </c>
-      <c r="C1" s="19" t="s">
+      <c r="C1" s="17" t="s">
         <v>336</v>
       </c>
-      <c r="D1" s="20"/>
-      <c r="E1" s="21"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="19"/>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="17">
+      <c r="A2" s="15">
         <v>1</v>
       </c>
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="17" t="s">
-        <v>4</v>
+      <c r="C2" s="15" t="s">
+        <v>355</v>
       </c>
       <c r="D2" t="str">
         <f>CONCATENATE("INSERT INTO ciudad( c_cod, c_desc) VALUES ( """,B2,""" , """,C2, """);")</f>
-        <v>INSERT INTO ciudad( c_cod, c_desc) VALUES ( "SAVR" , "Alto Río Senguer");</v>
+        <v>INSERT INTO ciudad( c_cod, c_desc) VALUES ( "SAVR" , "Alto Rio Senguer");</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -14792,7 +14867,7 @@
         <v>8</v>
       </c>
       <c r="D3" t="str">
-        <f t="shared" ref="D3:D5" si="0">CONCATENATE("INSERT INTO ciudad( c_cod, c_desc) VALUES ( """,B3,""" , """,C3, """);")</f>
+        <f t="shared" ref="D3:D66" si="0">CONCATENATE("INSERT INTO ciudad( c_cod, c_desc) VALUES ( """,B3,""" , """,C3, """);")</f>
         <v>INSERT INTO ciudad( c_cod, c_desc) VALUES ( "SAZA" , "Azul");</v>
       </c>
     </row>
@@ -14804,11 +14879,11 @@
         <v>13</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>12</v>
+        <v>356</v>
       </c>
       <c r="D4" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT INTO ciudad( c_cod, c_desc) VALUES ( "SAZB" , "Bahía Blanca");</v>
+        <v>INSERT INTO ciudad( c_cod, c_desc) VALUES ( "SAZB" , "Bahia Blanca");</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -14834,11 +14909,11 @@
         <v>19</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>18</v>
+        <v>357</v>
       </c>
       <c r="D6" t="str">
-        <f>CONCATENATE("INSERT INTO ciudad( c_cod, c_desc) VALUES ( """,B6,""" , """,C6, """);")</f>
-        <v>INSERT INTO ciudad( c_cod, c_desc) VALUES ( "SAZI" , "Bolívar");</v>
+        <f t="shared" si="0"/>
+        <v>INSERT INTO ciudad( c_cod, c_desc) VALUES ( "SAZI" , "Bolivar");</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -14852,7 +14927,7 @@
         <v>26</v>
       </c>
       <c r="D7" t="str">
-        <f>CONCATENATE("INSERT INTO ciudad( c_cod, c_desc) VALUES ( """,B7,""" , """,C7, """);")</f>
+        <f t="shared" si="0"/>
         <v>INSERT INTO ciudad( c_cod, c_desc) VALUES ( "SADO" , "Campo de Mayo");</v>
       </c>
     </row>
@@ -14867,7 +14942,7 @@
         <v>30</v>
       </c>
       <c r="D8" t="str">
-        <f>CONCATENATE("INSERT INTO ciudad( c_cod, c_desc) VALUES ( """,B8,""" , """,C8, """);")</f>
+        <f t="shared" si="0"/>
         <v>INSERT INTO ciudad( c_cod, c_desc) VALUES ( "SAHE" , "Caviahue");</v>
       </c>
     </row>
@@ -14882,7 +14957,7 @@
         <v>34</v>
       </c>
       <c r="D9" t="str">
-        <f>CONCATENATE("INSERT INTO ciudad( c_cod, c_desc) VALUES ( """,B9,""" , """,C9, """);")</f>
+        <f t="shared" si="0"/>
         <v>INSERT INTO ciudad( c_cod, c_desc) VALUES ( "SANW" , "Ceres");</v>
       </c>
     </row>
@@ -14897,7 +14972,7 @@
         <v>37</v>
       </c>
       <c r="D10" t="str">
-        <f>CONCATENATE("INSERT INTO ciudad( c_cod, c_desc) VALUES ( """,B10,""" , """,C10, """);")</f>
+        <f t="shared" si="0"/>
         <v>INSERT INTO ciudad( c_cod, c_desc) VALUES ( "SACT" , "Chamical");</v>
       </c>
     </row>
@@ -14912,7 +14987,7 @@
         <v>41</v>
       </c>
       <c r="D11" t="str">
-        <f>CONCATENATE("INSERT INTO ciudad( c_cod, c_desc) VALUES ( """,B11,""" , """,C11, """);")</f>
+        <f t="shared" si="0"/>
         <v>INSERT INTO ciudad( c_cod, c_desc) VALUES ( "SACP" , "Chepes");</v>
       </c>
     </row>
@@ -14927,7 +15002,7 @@
         <v>44</v>
       </c>
       <c r="D12" t="str">
-        <f>CONCATENATE("INSERT INTO ciudad( c_cod, c_desc) VALUES ( """,B12,""" , """,C12, """);")</f>
+        <f t="shared" si="0"/>
         <v>INSERT INTO ciudad( c_cod, c_desc) VALUES ( "SANO" , "Chilecito");</v>
       </c>
     </row>
@@ -14942,7 +15017,7 @@
         <v>47</v>
       </c>
       <c r="D13" t="str">
-        <f>CONCATENATE("INSERT INTO ciudad( c_cod, c_desc) VALUES ( """,B13,""" , """,C13, """);")</f>
+        <f t="shared" si="0"/>
         <v>INSERT INTO ciudad( c_cod, c_desc) VALUES ( "SATC" , "Clorinda");</v>
       </c>
     </row>
@@ -14957,7 +15032,7 @@
         <v>51</v>
       </c>
       <c r="D14" t="str">
-        <f>CONCATENATE("INSERT INTO ciudad( c_cod, c_desc) VALUES ( """,B14,""" , """,C14, """);")</f>
+        <f t="shared" si="0"/>
         <v>INSERT INTO ciudad( c_cod, c_desc) VALUES ( "SAVC" , "Comodoro Rivadavia");</v>
       </c>
     </row>
@@ -14969,11 +15044,11 @@
         <v>55</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>54</v>
+        <v>373</v>
       </c>
       <c r="D15" t="str">
-        <f>CONCATENATE("INSERT INTO ciudad( c_cod, c_desc) VALUES ( """,B15,""" , """,C15, """);")</f>
-        <v>INSERT INTO ciudad( c_cod, c_desc) VALUES ( "SACO" , "Córdoba");</v>
+        <f t="shared" si="0"/>
+        <v>INSERT INTO ciudad( c_cod, c_desc) VALUES ( "SACO" , "Cordoba");</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -14987,7 +15062,7 @@
         <v>57</v>
       </c>
       <c r="D16" t="str">
-        <f>CONCATENATE("INSERT INTO ciudad( c_cod, c_desc) VALUES ( """,B16,""" , """,C16, """);")</f>
+        <f t="shared" si="0"/>
         <v>INSERT INTO ciudad( c_cod, c_desc) VALUES ( "SAAC" , "Concordia");</v>
       </c>
     </row>
@@ -14999,11 +15074,11 @@
         <v>62</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>61</v>
+        <v>367</v>
       </c>
       <c r="D17" t="str">
-        <f>CONCATENATE("INSERT INTO ciudad( c_cod, c_desc) VALUES ( """,B17,""" , """,C17, """);")</f>
-        <v>INSERT INTO ciudad( c_cod, c_desc) VALUES ( "SAZC" , "Coronel Suárez");</v>
+        <f t="shared" si="0"/>
+        <v>INSERT INTO ciudad( c_cod, c_desc) VALUES ( "SAZC" , "Coronel Suarez");</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -15017,7 +15092,7 @@
         <v>64</v>
       </c>
       <c r="D18" t="str">
-        <f>CONCATENATE("INSERT INTO ciudad( c_cod, c_desc) VALUES ( """,B18,""" , """,C18, """);")</f>
+        <f t="shared" si="0"/>
         <v>INSERT INTO ciudad( c_cod, c_desc) VALUES ( "SARC" , "Corrientes");</v>
       </c>
     </row>
@@ -15029,11 +15104,11 @@
         <v>68</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>67</v>
+        <v>378</v>
       </c>
       <c r="D19" t="str">
-        <f>CONCATENATE("INSERT INTO ciudad( c_cod, c_desc) VALUES ( """,B19,""" , """,C19, """);")</f>
-        <v>INSERT INTO ciudad( c_cod, c_desc) VALUES ( "SATU" , "Curuzú Cuatiá");</v>
+        <f t="shared" si="0"/>
+        <v>INSERT INTO ciudad( c_cod, c_desc) VALUES ( "SATU" , "Curuzu Cuatia");</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -15047,7 +15122,7 @@
         <v>70</v>
       </c>
       <c r="D20" t="str">
-        <f>CONCATENATE("INSERT INTO ciudad( c_cod, c_desc) VALUES ( """,B20,""" , """,C20, """);")</f>
+        <f t="shared" si="0"/>
         <v>INSERT INTO ciudad( c_cod, c_desc) VALUES ( "SAZW" , "Cutral-Co");</v>
       </c>
     </row>
@@ -15062,7 +15137,7 @@
         <v>73</v>
       </c>
       <c r="D21" t="str">
-        <f>CONCATENATE("INSERT INTO ciudad( c_cod, c_desc) VALUES ( """,B21,""" , """,C21, """);")</f>
+        <f t="shared" si="0"/>
         <v>INSERT INTO ciudad( c_cod, c_desc) VALUES ( "SAZD" , "Dolores");</v>
       </c>
     </row>
@@ -15077,7 +15152,7 @@
         <v>76</v>
       </c>
       <c r="D22" t="str">
-        <f>CONCATENATE("INSERT INTO ciudad( c_cod, c_desc) VALUES ( """,B22,""" , """,C22, """);")</f>
+        <f t="shared" si="0"/>
         <v>INSERT INTO ciudad( c_cod, c_desc) VALUES ( "SADD" , "Don Torcuato");</v>
       </c>
     </row>
@@ -15089,11 +15164,11 @@
         <v>81</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>79</v>
+        <v>374</v>
       </c>
       <c r="D23" t="str">
-        <f>CONCATENATE("INSERT INTO ciudad( c_cod, c_desc) VALUES ( """,B23,""" , """,C23, """);")</f>
-        <v>INSERT INTO ciudad( c_cod, c_desc) VALUES ( "SAVB" , "El Bolsón");</v>
+        <f t="shared" si="0"/>
+        <v>INSERT INTO ciudad( c_cod, c_desc) VALUES ( "SAVB" , "El Bolson");</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -15107,7 +15182,7 @@
         <v>83</v>
       </c>
       <c r="D24" t="str">
-        <f>CONCATENATE("INSERT INTO ciudad( c_cod, c_desc) VALUES ( """,B24,""" , """,C24, """);")</f>
+        <f t="shared" si="0"/>
         <v>INSERT INTO ciudad( c_cod, c_desc) VALUES ( "SAWC" , "El Calafate");</v>
       </c>
     </row>
@@ -15122,7 +15197,7 @@
         <v>83</v>
       </c>
       <c r="D25" t="str">
-        <f>CONCATENATE("INSERT INTO ciudad( c_cod, c_desc) VALUES ( """,B25,""" , """,C25, """);")</f>
+        <f t="shared" si="0"/>
         <v>INSERT INTO ciudad( c_cod, c_desc) VALUES ( "SAWA" , "El Calafate");</v>
       </c>
     </row>
@@ -15137,7 +15212,7 @@
         <v>88</v>
       </c>
       <c r="D26" t="str">
-        <f>CONCATENATE("INSERT INTO ciudad( c_cod, c_desc) VALUES ( """,B26,""" , """,C26, """);")</f>
+        <f t="shared" si="0"/>
         <v>INSERT INTO ciudad( c_cod, c_desc) VALUES ( "SADP" , "El Palomar");</v>
       </c>
     </row>
@@ -15152,7 +15227,7 @@
         <v>91</v>
       </c>
       <c r="D27" t="str">
-        <f>CONCATENATE("INSERT INTO ciudad( c_cod, c_desc) VALUES ( """,B27,""" , """,C27, """);")</f>
+        <f t="shared" si="0"/>
         <v>INSERT INTO ciudad( c_cod, c_desc) VALUES ( "SAVE" , "Esquel");</v>
       </c>
     </row>
@@ -15167,7 +15242,7 @@
         <v>94</v>
       </c>
       <c r="D28" t="str">
-        <f>CONCATENATE("INSERT INTO ciudad( c_cod, c_desc) VALUES ( """,B28,""" , """,C28, """);")</f>
+        <f t="shared" si="0"/>
         <v>INSERT INTO ciudad( c_cod, c_desc) VALUES ( "SAEZ" , "Ezeiza");</v>
       </c>
     </row>
@@ -15182,7 +15257,7 @@
         <v>48</v>
       </c>
       <c r="D29" t="str">
-        <f>CONCATENATE("INSERT INTO ciudad( c_cod, c_desc) VALUES ( """,B29,""" , """,C29, """);")</f>
+        <f t="shared" si="0"/>
         <v>INSERT INTO ciudad( c_cod, c_desc) VALUES ( "SARF" , "Formosa");</v>
       </c>
     </row>
@@ -15197,7 +15272,7 @@
         <v>99</v>
       </c>
       <c r="D30" t="str">
-        <f>CONCATENATE("INSERT INTO ciudad( c_cod, c_desc) VALUES ( """,B30,""" , """,C30, """);")</f>
+        <f t="shared" si="0"/>
         <v>INSERT INTO ciudad( c_cod, c_desc) VALUES ( "SAMA" , "General Alvear");</v>
       </c>
     </row>
@@ -15212,7 +15287,7 @@
         <v>103</v>
       </c>
       <c r="D31" t="str">
-        <f>CONCATENATE("INSERT INTO ciudad( c_cod, c_desc) VALUES ( """,B31,""" , """,C31, """);")</f>
+        <f t="shared" si="0"/>
         <v>INSERT INTO ciudad( c_cod, c_desc) VALUES ( "SAZG" , "General Pico");</v>
       </c>
     </row>
@@ -15227,7 +15302,7 @@
         <v>107</v>
       </c>
       <c r="D32" t="str">
-        <f>CONCATENATE("INSERT INTO ciudad( c_cod, c_desc) VALUES ( """,B32,""" , """,C32, """);")</f>
+        <f t="shared" si="0"/>
         <v>INSERT INTO ciudad( c_cod, c_desc) VALUES ( "SAHR" , "General Roca");</v>
       </c>
     </row>
@@ -15242,7 +15317,7 @@
         <v>110</v>
       </c>
       <c r="D33" t="str">
-        <f>CONCATENATE("INSERT INTO ciudad( c_cod, c_desc) VALUES ( """,B33,""" , """,C33, """);")</f>
+        <f t="shared" si="0"/>
         <v>INSERT INTO ciudad( c_cod, c_desc) VALUES ( "SAVJ" , "Ingeniero Jacobacci");</v>
       </c>
     </row>
@@ -15254,11 +15329,11 @@
         <v>114</v>
       </c>
       <c r="C34" s="9" t="s">
-        <v>113</v>
+        <v>358</v>
       </c>
       <c r="D34" t="str">
-        <f>CONCATENATE("INSERT INTO ciudad( c_cod, c_desc) VALUES ( """,B34,""" , """,C34, """);")</f>
-        <v>INSERT INTO ciudad( c_cod, c_desc) VALUES ( "SAAK" , "Isla Martín García");</v>
+        <f t="shared" si="0"/>
+        <v>INSERT INTO ciudad( c_cod, c_desc) VALUES ( "SAAK" , "Isla Martin Garcia");</v>
       </c>
     </row>
     <row r="35" spans="1:4">
@@ -15269,11 +15344,11 @@
         <v>117</v>
       </c>
       <c r="C35" s="9" t="s">
-        <v>116</v>
+        <v>371</v>
       </c>
       <c r="D35" t="str">
-        <f>CONCATENATE("INSERT INTO ciudad( c_cod, c_desc) VALUES ( """,B35,""" , """,C35, """);")</f>
-        <v>INSERT INTO ciudad( c_cod, c_desc) VALUES ( "SADJ" , "José C. Paz");</v>
+        <f t="shared" si="0"/>
+        <v>INSERT INTO ciudad( c_cod, c_desc) VALUES ( "SADJ" , "Jose C. Paz");</v>
       </c>
     </row>
     <row r="36" spans="1:4">
@@ -15284,11 +15359,11 @@
         <v>120</v>
       </c>
       <c r="C36" s="9" t="s">
-        <v>119</v>
+        <v>359</v>
       </c>
       <c r="D36" t="str">
-        <f>CONCATENATE("INSERT INTO ciudad( c_cod, c_desc) VALUES ( """,B36,""" , """,C36, """);")</f>
-        <v>INSERT INTO ciudad( c_cod, c_desc) VALUES ( "SAAJ" , "Junín");</v>
+        <f t="shared" si="0"/>
+        <v>INSERT INTO ciudad( c_cod, c_desc) VALUES ( "SAAJ" , "Junin");</v>
       </c>
     </row>
     <row r="37" spans="1:4">
@@ -15302,7 +15377,7 @@
         <v>122</v>
       </c>
       <c r="D37" t="str">
-        <f>CONCATENATE("INSERT INTO ciudad( c_cod, c_desc) VALUES ( """,B37,""" , """,C37, """);")</f>
+        <f t="shared" si="0"/>
         <v>INSERT INTO ciudad( c_cod, c_desc) VALUES ( "SAOL" , "Laboulaye");</v>
       </c>
     </row>
@@ -15317,7 +15392,7 @@
         <v>125</v>
       </c>
       <c r="D38" t="str">
-        <f>CONCATENATE("INSERT INTO ciudad( c_cod, c_desc) VALUES ( """,B38,""" , """,C38, """);")</f>
+        <f t="shared" si="0"/>
         <v>INSERT INTO ciudad( c_cod, c_desc) VALUES ( "SACC" , "La Cumbre");</v>
       </c>
     </row>
@@ -15332,7 +15407,7 @@
         <v>128</v>
       </c>
       <c r="D39" t="str">
-        <f>CONCATENATE("INSERT INTO ciudad( c_cod, c_desc) VALUES ( """,B39,""" , """,C39, """);")</f>
+        <f t="shared" si="0"/>
         <v>INSERT INTO ciudad( c_cod, c_desc) VALUES ( "SADL" , "La Plata");</v>
       </c>
     </row>
@@ -15347,7 +15422,7 @@
         <v>38</v>
       </c>
       <c r="D40" t="str">
-        <f>CONCATENATE("INSERT INTO ciudad( c_cod, c_desc) VALUES ( """,B40,""" , """,C40, """);")</f>
+        <f t="shared" si="0"/>
         <v>INSERT INTO ciudad( c_cod, c_desc) VALUES ( "SANL" , "La Rioja");</v>
       </c>
     </row>
@@ -15362,7 +15437,7 @@
         <v>133</v>
       </c>
       <c r="D41" t="str">
-        <f>CONCATENATE("INSERT INTO ciudad( c_cod, c_desc) VALUES ( """,B41,""" , """,C41, """);")</f>
+        <f t="shared" si="0"/>
         <v>INSERT INTO ciudad( c_cod, c_desc) VALUES ( "SAVH" , "Las Heras");</v>
       </c>
     </row>
@@ -15377,7 +15452,7 @@
         <v>136</v>
       </c>
       <c r="D42" t="str">
-        <f>CONCATENATE("INSERT INTO ciudad( c_cod, c_desc) VALUES ( """,B42,""" , """,C42, """);")</f>
+        <f t="shared" si="0"/>
         <v>INSERT INTO ciudad( c_cod, c_desc) VALUES ( "SATK" , "Las Lomitas");</v>
       </c>
     </row>
@@ -15392,7 +15467,7 @@
         <v>139</v>
       </c>
       <c r="D43" t="str">
-        <f>CONCATENATE("INSERT INTO ciudad( c_cod, c_desc) VALUES ( """,B43,""" , """,C43, """);")</f>
+        <f t="shared" si="0"/>
         <v>INSERT INTO ciudad( c_cod, c_desc) VALUES ( "SAMM" , "Malargüe");</v>
       </c>
     </row>
@@ -15407,7 +15482,7 @@
         <v>142</v>
       </c>
       <c r="D44" t="str">
-        <f>CONCATENATE("INSERT INTO ciudad( c_cod, c_desc) VALUES ( """,B44,""" , """,C44, """);")</f>
+        <f t="shared" si="0"/>
         <v>INSERT INTO ciudad( c_cod, c_desc) VALUES ( "SAZM" , "Mar del Plata");</v>
       </c>
     </row>
@@ -15422,7 +15497,7 @@
         <v>100</v>
       </c>
       <c r="D45" t="str">
-        <f>CONCATENATE("INSERT INTO ciudad( c_cod, c_desc) VALUES ( """,B45,""" , """,C45, """);")</f>
+        <f t="shared" si="0"/>
         <v>INSERT INTO ciudad( c_cod, c_desc) VALUES ( "SAME" , "Mendoza");</v>
       </c>
     </row>
@@ -15437,7 +15512,7 @@
         <v>147</v>
       </c>
       <c r="D46" t="str">
-        <f>CONCATENATE("INSERT INTO ciudad( c_cod, c_desc) VALUES ( """,B46,""" , """,C46, """);")</f>
+        <f t="shared" si="0"/>
         <v>INSERT INTO ciudad( c_cod, c_desc) VALUES ( "SAOS" , "Merlo");</v>
       </c>
     </row>
@@ -15452,7 +15527,7 @@
         <v>151</v>
       </c>
       <c r="D47" t="str">
-        <f>CONCATENATE("INSERT INTO ciudad( c_cod, c_desc) VALUES ( """,B47,""" , """,C47, """);")</f>
+        <f t="shared" si="0"/>
         <v>INSERT INTO ciudad( c_cod, c_desc) VALUES ( "SAEM" , "Miramar");</v>
       </c>
     </row>
@@ -15467,7 +15542,7 @@
         <v>154</v>
       </c>
       <c r="D48" t="str">
-        <f>CONCATENATE("INSERT INTO ciudad( c_cod, c_desc) VALUES ( """,B48,""" , """,C48, """);")</f>
+        <f t="shared" si="0"/>
         <v>INSERT INTO ciudad( c_cod, c_desc) VALUES ( "SARM" , "Monte Caseros");</v>
       </c>
     </row>
@@ -15479,11 +15554,11 @@
         <v>158</v>
       </c>
       <c r="C49" s="9" t="s">
-        <v>157</v>
+        <v>375</v>
       </c>
       <c r="D49" t="str">
-        <f>CONCATENATE("INSERT INTO ciudad( c_cod, c_desc) VALUES ( """,B49,""" , """,C49, """);")</f>
-        <v>INSERT INTO ciudad( c_cod, c_desc) VALUES ( "SADM" , "Morón");</v>
+        <f t="shared" si="0"/>
+        <v>INSERT INTO ciudad( c_cod, c_desc) VALUES ( "SADM" , "Moron");</v>
       </c>
     </row>
     <row r="50" spans="1:4">
@@ -15497,7 +15572,7 @@
         <v>160</v>
       </c>
       <c r="D50" t="str">
-        <f>CONCATENATE("INSERT INTO ciudad( c_cod, c_desc) VALUES ( """,B50,""" , """,C50, """);")</f>
+        <f t="shared" si="0"/>
         <v>INSERT INTO ciudad( c_cod, c_desc) VALUES ( "SAZO" , "Necochea");</v>
       </c>
     </row>
@@ -15509,11 +15584,11 @@
         <v>163</v>
       </c>
       <c r="C51" s="9" t="s">
-        <v>31</v>
+        <v>372</v>
       </c>
       <c r="D51" t="str">
-        <f>CONCATENATE("INSERT INTO ciudad( c_cod, c_desc) VALUES ( """,B51,""" , """,C51, """);")</f>
-        <v>INSERT INTO ciudad( c_cod, c_desc) VALUES ( "SAZN" , "Neuquén");</v>
+        <f t="shared" si="0"/>
+        <v>INSERT INTO ciudad( c_cod, c_desc) VALUES ( "SAZN" , "Neuquen");</v>
       </c>
     </row>
     <row r="52" spans="1:4">
@@ -15524,11 +15599,11 @@
         <v>166</v>
       </c>
       <c r="C52" s="9" t="s">
-        <v>165</v>
+        <v>360</v>
       </c>
       <c r="D52" t="str">
-        <f>CONCATENATE("INSERT INTO ciudad( c_cod, c_desc) VALUES ( """,B52,""" , """,C52, """);")</f>
-        <v>INSERT INTO ciudad( c_cod, c_desc) VALUES ( "SAZF" , "Olavarría");</v>
+        <f t="shared" si="0"/>
+        <v>INSERT INTO ciudad( c_cod, c_desc) VALUES ( "SAZF" , "Olavarria");</v>
       </c>
     </row>
     <row r="53" spans="1:4">
@@ -15539,11 +15614,11 @@
         <v>169</v>
       </c>
       <c r="C53" s="9" t="s">
-        <v>168</v>
+        <v>368</v>
       </c>
       <c r="D53" t="str">
-        <f>CONCATENATE("INSERT INTO ciudad( c_cod, c_desc) VALUES ( """,B53,""" , """,C53, """);")</f>
-        <v>INSERT INTO ciudad( c_cod, c_desc) VALUES ( "SAAP" , "Paraná");</v>
+        <f t="shared" si="0"/>
+        <v>INSERT INTO ciudad( c_cod, c_desc) VALUES ( "SAAP" , "Parana");</v>
       </c>
     </row>
     <row r="54" spans="1:4">
@@ -15557,7 +15632,7 @@
         <v>171</v>
       </c>
       <c r="D54" t="str">
-        <f>CONCATENATE("INSERT INTO ciudad( c_cod, c_desc) VALUES ( """,B54,""" , """,C54, """);")</f>
+        <f t="shared" si="0"/>
         <v>INSERT INTO ciudad( c_cod, c_desc) VALUES ( "SARL" , "Paso de los Libres");</v>
       </c>
     </row>
@@ -15569,11 +15644,11 @@
         <v>175</v>
       </c>
       <c r="C55" s="9" t="s">
-        <v>174</v>
+        <v>376</v>
       </c>
       <c r="D55" t="str">
-        <f>CONCATENATE("INSERT INTO ciudad( c_cod, c_desc) VALUES ( """,B55,""" , """,C55, """);")</f>
-        <v>INSERT INTO ciudad( c_cod, c_desc) VALUES ( "SAZP" , "Pehuajó");</v>
+        <f t="shared" si="0"/>
+        <v>INSERT INTO ciudad( c_cod, c_desc) VALUES ( "SAZP" , "Pehuajo");</v>
       </c>
     </row>
     <row r="56" spans="1:4">
@@ -15587,7 +15662,7 @@
         <v>177</v>
       </c>
       <c r="D56" t="str">
-        <f>CONCATENATE("INSERT INTO ciudad( c_cod, c_desc) VALUES ( """,B56,""" , """,C56, """);")</f>
+        <f t="shared" si="0"/>
         <v>INSERT INTO ciudad( c_cod, c_desc) VALUES ( "SASJ" , "Perico");</v>
       </c>
     </row>
@@ -15602,7 +15677,7 @@
         <v>181</v>
       </c>
       <c r="D57" t="str">
-        <f>CONCATENATE("INSERT INTO ciudad( c_cod, c_desc) VALUES ( """,B57,""" , """,C57, """);")</f>
+        <f t="shared" si="0"/>
         <v>INSERT INTO ciudad( c_cod, c_desc) VALUES ( "SAWP" , "Perito Moreno");</v>
       </c>
     </row>
@@ -15617,7 +15692,7 @@
         <v>184</v>
       </c>
       <c r="D58" t="str">
-        <f>CONCATENATE("INSERT INTO ciudad( c_cod, c_desc) VALUES ( """,B58,""" , """,C58, """);")</f>
+        <f t="shared" si="0"/>
         <v>INSERT INTO ciudad( c_cod, c_desc) VALUES ( "SARP" , "Posadas");</v>
       </c>
     </row>
@@ -15632,7 +15707,7 @@
         <v>188</v>
       </c>
       <c r="D59" t="str">
-        <f>CONCATENATE("INSERT INTO ciudad( c_cod, c_desc) VALUES ( """,B59,""" , """,C59, """);")</f>
+        <f t="shared" si="0"/>
         <v>INSERT INTO ciudad( c_cod, c_desc) VALUES ( "SAWD" , "Puerto Deseado");</v>
       </c>
     </row>
@@ -15644,11 +15719,11 @@
         <v>192</v>
       </c>
       <c r="C60" s="9" t="s">
-        <v>191</v>
+        <v>379</v>
       </c>
       <c r="D60" t="str">
-        <f>CONCATENATE("INSERT INTO ciudad( c_cod, c_desc) VALUES ( """,B60,""" , """,C60, """);")</f>
-        <v>INSERT INTO ciudad( c_cod, c_desc) VALUES ( "SARI" , "Puerto Iguazú");</v>
+        <f t="shared" si="0"/>
+        <v>INSERT INTO ciudad( c_cod, c_desc) VALUES ( "SARI" , "Puerto Iguazu");</v>
       </c>
     </row>
     <row r="61" spans="1:4">
@@ -15662,7 +15737,7 @@
         <v>194</v>
       </c>
       <c r="D61" t="str">
-        <f>CONCATENATE("INSERT INTO ciudad( c_cod, c_desc) VALUES ( """,B61,""" , """,C61, """);")</f>
+        <f t="shared" si="0"/>
         <v>INSERT INTO ciudad( c_cod, c_desc) VALUES ( "SAVY" , "Puerto Madryn");</v>
       </c>
     </row>
@@ -15674,11 +15749,11 @@
         <v>198</v>
       </c>
       <c r="C62" s="9" t="s">
-        <v>197</v>
+        <v>369</v>
       </c>
       <c r="D62" t="str">
-        <f>CONCATENATE("INSERT INTO ciudad( c_cod, c_desc) VALUES ( """,B62,""" , """,C62, """);")</f>
-        <v>INSERT INTO ciudad( c_cod, c_desc) VALUES ( "SAWJ" , "Puerto San Julián");</v>
+        <f t="shared" si="0"/>
+        <v>INSERT INTO ciudad( c_cod, c_desc) VALUES ( "SAWJ" , "Puerto San Julian");</v>
       </c>
     </row>
     <row r="63" spans="1:4">
@@ -15692,7 +15767,7 @@
         <v>200</v>
       </c>
       <c r="D63" t="str">
-        <f>CONCATENATE("INSERT INTO ciudad( c_cod, c_desc) VALUES ( """,B63,""" , """,C63, """);")</f>
+        <f t="shared" si="0"/>
         <v>INSERT INTO ciudad( c_cod, c_desc) VALUES ( "SAWU" , "Puerto Santa Cruz");</v>
       </c>
     </row>
@@ -15707,7 +15782,7 @@
         <v>203</v>
       </c>
       <c r="D64" t="str">
-        <f>CONCATENATE("INSERT INTO ciudad( c_cod, c_desc) VALUES ( """,B64,""" , """,C64, """);")</f>
+        <f t="shared" si="0"/>
         <v>INSERT INTO ciudad( c_cod, c_desc) VALUES ( "SASA" , "Presidencia Roque Saenz Peña");</v>
       </c>
     </row>
@@ -15722,7 +15797,7 @@
         <v>207</v>
       </c>
       <c r="D65" t="str">
-        <f>CONCATENATE("INSERT INTO ciudad( c_cod, c_desc) VALUES ( """,B65,""" , """,C65, """);")</f>
+        <f t="shared" si="0"/>
         <v>INSERT INTO ciudad( c_cod, c_desc) VALUES ( "SATR" , "Reconquista");</v>
       </c>
     </row>
@@ -15737,7 +15812,7 @@
         <v>210</v>
       </c>
       <c r="D66" t="str">
-        <f>CONCATENATE("INSERT INTO ciudad( c_cod, c_desc) VALUES ( """,B66,""" , """,C66, """);")</f>
+        <f t="shared" si="0"/>
         <v>INSERT INTO ciudad( c_cod, c_desc) VALUES ( "SARE" , "Resistencia");</v>
       </c>
     </row>
@@ -15749,11 +15824,11 @@
         <v>214</v>
       </c>
       <c r="C67" s="9" t="s">
-        <v>213</v>
+        <v>361</v>
       </c>
       <c r="D67" t="str">
         <f t="shared" ref="D67:D98" si="1">CONCATENATE("INSERT INTO ciudad( c_cod, c_desc) VALUES ( """,B67,""" , """,C67, """);")</f>
-        <v>INSERT INTO ciudad( c_cod, c_desc) VALUES ( "SAOC" , "Río Cuarto");</v>
+        <v>INSERT INTO ciudad( c_cod, c_desc) VALUES ( "SAOC" , "Rio Cuarto");</v>
       </c>
     </row>
     <row r="68" spans="1:4">
@@ -15764,11 +15839,11 @@
         <v>217</v>
       </c>
       <c r="C68" s="9" t="s">
-        <v>216</v>
+        <v>362</v>
       </c>
       <c r="D68" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO ciudad( c_cod, c_desc) VALUES ( "SAWG" , "Río Gallegos");</v>
+        <v>INSERT INTO ciudad( c_cod, c_desc) VALUES ( "SAWG" , "Rio Gallegos");</v>
       </c>
     </row>
     <row r="69" spans="1:4">
@@ -15779,11 +15854,11 @@
         <v>221</v>
       </c>
       <c r="C69" s="9" t="s">
-        <v>219</v>
+        <v>363</v>
       </c>
       <c r="D69" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO ciudad( c_cod, c_desc) VALUES ( "SAWE" , "Río Grande");</v>
+        <v>INSERT INTO ciudad( c_cod, c_desc) VALUES ( "SAWE" , "Rio Grande");</v>
       </c>
     </row>
     <row r="70" spans="1:4">
@@ -15794,11 +15869,11 @@
         <v>223</v>
       </c>
       <c r="C70" s="9" t="s">
-        <v>307</v>
+        <v>364</v>
       </c>
       <c r="D70" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO ciudad( c_cod, c_desc) VALUES ( "SAWT" , "Río Turbio");</v>
+        <v>INSERT INTO ciudad( c_cod, c_desc) VALUES ( "SAWT" , "Rio Turbio");</v>
       </c>
     </row>
     <row r="71" spans="1:4">
@@ -15899,11 +15974,11 @@
         <v>244</v>
       </c>
       <c r="C77" s="9" t="s">
-        <v>243</v>
+        <v>377</v>
       </c>
       <c r="D77" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO ciudad( c_cod, c_desc) VALUES ( "SASO" , "San Ramón de la Nueva Orán");</v>
+        <v>INSERT INTO ciudad( c_cod, c_desc) VALUES ( "SASO" , "San Ramon de la Nueva Oran");</v>
       </c>
     </row>
     <row r="78" spans="1:4">
@@ -15929,11 +16004,11 @@
         <v>251</v>
       </c>
       <c r="C79" s="9" t="s">
-        <v>249</v>
+        <v>370</v>
       </c>
       <c r="D79" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO ciudad( c_cod, c_desc) VALUES ( "SANT" , "San Miguel de Tucumán");</v>
+        <v>INSERT INTO ciudad( c_cod, c_desc) VALUES ( "SANT" , "San Miguel de Tucuman");</v>
       </c>
     </row>
     <row r="80" spans="1:4">
@@ -15989,11 +16064,11 @@
         <v>263</v>
       </c>
       <c r="C83" s="9" t="s">
-        <v>262</v>
+        <v>365</v>
       </c>
       <c r="D83" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO ciudad( c_cod, c_desc) VALUES ( "SAZY" , "San Martín de los Andes");</v>
+        <v>INSERT INTO ciudad( c_cod, c_desc) VALUES ( "SAZY" , "San Martin de los Andes");</v>
       </c>
     </row>
     <row r="84" spans="1:4">
@@ -16064,11 +16139,11 @@
         <v>278</v>
       </c>
       <c r="C88" s="9" t="s">
-        <v>277</v>
+        <v>366</v>
       </c>
       <c r="D88" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO ciudad( c_cod, c_desc) VALUES ( "SANR" , "Termas de Río Hondo");</v>
+        <v>INSERT INTO ciudad( c_cod, c_desc) VALUES ( "SANR" , "Termas de Rio Hondo");</v>
       </c>
     </row>
     <row r="89" spans="1:4">
@@ -16210,7 +16285,7 @@
       <c r="A98" s="9">
         <v>97</v>
       </c>
-      <c r="B98" s="16" t="s">
+      <c r="B98" s="14" t="s">
         <v>21</v>
       </c>
       <c r="C98" s="9" t="s">
@@ -16251,23 +16326,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="22"/>
-      <c r="B1" s="22" t="s">
+      <c r="A1" s="20"/>
+      <c r="B1" s="20" t="s">
         <v>337</v>
       </c>
-      <c r="C1" s="22" t="s">
+      <c r="C1" s="20" t="s">
         <v>338</v>
       </c>
-      <c r="D1" s="22" t="s">
+      <c r="D1" s="20" t="s">
         <v>339</v>
       </c>
-      <c r="E1" s="22" t="s">
+      <c r="E1" s="20" t="s">
         <v>340</v>
       </c>
-      <c r="F1" s="22" t="s">
+      <c r="F1" s="20" t="s">
         <v>341</v>
       </c>
-      <c r="G1" s="22" t="s">
+      <c r="G1" s="20" t="s">
         <v>342</v>
       </c>
     </row>
@@ -22520,7 +22595,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+    <sheetView topLeftCell="G1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="H9" sqref="H9"/>
     </sheetView>
@@ -22536,23 +22611,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="23"/>
-      <c r="B1" s="23" t="s">
+      <c r="A1" s="21"/>
+      <c r="B1" s="21" t="s">
         <v>339</v>
       </c>
-      <c r="C1" s="23" t="s">
+      <c r="C1" s="21" t="s">
         <v>350</v>
       </c>
-      <c r="D1" s="23" t="s">
+      <c r="D1" s="21" t="s">
         <v>351</v>
       </c>
-      <c r="E1" s="23" t="s">
+      <c r="E1" s="21" t="s">
         <v>352</v>
       </c>
-      <c r="F1" s="23" t="s">
+      <c r="F1" s="21" t="s">
         <v>353</v>
       </c>
-      <c r="G1" s="23" t="s">
+      <c r="G1" s="21" t="s">
         <v>354</v>
       </c>
     </row>

</xml_diff>